<commit_message>
.xlsx graph title modified
</commit_message>
<xml_diff>
--- a/DP/fet_03v3/nfet_03v3_dcop_ss/nfet_03v3_dcop_ss.xlsx
+++ b/DP/fet_03v3/nfet_03v3_dcop_ss/nfet_03v3_dcop_ss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72bddbd06fd932c9/共有/iic-osic/nfet_03v3_dcop_ss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{A49C1FF0-87D1-4D93-BBBB-67AD3120EEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D59EB6-AA8E-4A6F-94AA-715E0CD794E6}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{A49C1FF0-87D1-4D93-BBBB-67AD3120EEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C345D756-CE7F-4ABD-9568-DA0011FE7C31}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="0" windowWidth="12600" windowHeight="15150" firstSheet="1" activeTab="1" xr2:uid="{48AB8966-9D5B-409D-ADE7-0D00F9BC5817}"/>
+    <workbookView xWindow="0" yWindow="7575" windowWidth="12600" windowHeight="7575" firstSheet="1" activeTab="1" xr2:uid="{48AB8966-9D5B-409D-ADE7-0D00F9BC5817}"/>
   </bookViews>
   <sheets>
     <sheet name="nfet_03v3_dcop_ss" sheetId="2" r:id="rId1"/>
@@ -3280,7 +3280,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>Cgg (nfet_03v3) PVT=ff</a:t>
+              <a:t>Cgg (nfet_03v3) PVT=ss</a:t>
             </a:r>
             <a:endParaRPr lang="ja-JP" altLang="en-US"/>
           </a:p>
@@ -4928,6 +4928,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{8BDBEA14-94A1-480A-B335-C8650CC3BB50}" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8">
@@ -54183,7 +54187,9 @@
   </sheetPr>
   <dimension ref="B1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>